<commit_message>
- cover more cases in the test data  - make script more robust  - add column 'gui_attributes' to template  - update docs  - add unit tests for excel2properties
</commit_message>
<xml_diff>
--- a/testdata/Resources.xlsx
+++ b/testdata/Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrivoal/Git-projets/medialitterature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E269DD2A-5CC0-834D-8DA7-E68A09DDFCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E8D7E5C-644C-7048-A9EF-6D8ABA5E2AD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25480" yWindow="500" windowWidth="25720" windowHeight="28300" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="8" r:id="rId1"/>
@@ -20,6 +20,14 @@
     <sheet name="FamilyMember" sheetId="5" r:id="rId5"/>
     <sheet name="MentionedPerson" sheetId="6" r:id="rId6"/>
     <sheet name="Alias" sheetId="7" r:id="rId7"/>
+    <sheet name="Image" sheetId="9" r:id="rId8"/>
+    <sheet name="Video" sheetId="10" r:id="rId9"/>
+    <sheet name="Audio" sheetId="11" r:id="rId10"/>
+    <sheet name="ZIP" sheetId="12" r:id="rId11"/>
+    <sheet name="PDFDocument" sheetId="13" r:id="rId12"/>
+    <sheet name="Annotation" sheetId="14" r:id="rId13"/>
+    <sheet name="LinkObject" sheetId="15" r:id="rId14"/>
+    <sheet name="RegionOfImage" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="150">
   <si>
     <t>Cardinality</t>
   </si>
@@ -93,24 +101,12 @@
     <t>Resource</t>
   </si>
   <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>property</t>
   </si>
   <si>
     <t>cardinality</t>
   </si>
   <si>
-    <t>isTitle</t>
-  </si>
-  <si>
-    <t>isTitleInEnglish</t>
-  </si>
-  <si>
     <t>isTitleInFrench</t>
   </si>
   <si>
@@ -132,12 +128,6 @@
     <t>isPlaceRelatedTo</t>
   </si>
   <si>
-    <t>GenericAnthroponym</t>
-  </si>
-  <si>
-    <t>Generic anthroponym</t>
-  </si>
-  <si>
     <t>isGenericAnthroponym</t>
   </si>
   <si>
@@ -249,12 +239,6 @@
     <t>comment_fr</t>
   </si>
   <si>
-    <t>I had established myself for several months in a central city in one of our southern departments, whose shore is bathed by the Mediterranean, and I was desirous of purchasing a country place in that marvellously picturesque land. </t>
-  </si>
-  <si>
-    <t>I had already looked at several pieces of property when, one day, the notary, who had been giving me some necessary directions for one of my explorations, said to me:</t>
-  </si>
-  <si>
     <t>I have just received notice that at about eight leagues from here, in one of the most beautiful situations in the world, neither too far nor too near to the sea, there is a country house for sale.</t>
   </si>
   <si>
@@ -345,9 +329,6 @@
     <t>Membro della famiglia</t>
   </si>
   <si>
-    <t>Persona menzionata</t>
-  </si>
-  <si>
     <t>Eigentümer</t>
   </si>
   <si>
@@ -361,6 +342,153 @@
   </si>
   <si>
     <t>Erwähnte Person</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Bild</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>MovingImageRepresentation</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>AudioRepresentation</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>ArchiveRepresentation</t>
+  </si>
+  <si>
+    <t>DocumentRepresentation</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>LinkObj</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>1-N</t>
+  </si>
+  <si>
+    <t>0-N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">isTitle  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> isTitleInEnglish </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  GenericAnthroponym  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic anthroponym </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Owner  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  I had established myself for several months in a central city in one of our southern departments, whose shore is bathed by the Mediterranean, and I was desirous of purchasing a country place in that marvellously picturesque land. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">I had already looked at several pieces of property when, one day, the notary, who had been giving me some necessary directions for one of my explorations, said to me:  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alias  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Persona menzionata  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resource</t>
+  </si>
+  <si>
+    <t>LinkObject</t>
+  </si>
+  <si>
+    <t>Link Object</t>
+  </si>
+  <si>
+    <t>RegionOfImage</t>
+  </si>
+  <si>
+    <t>Region of an image</t>
+  </si>
+  <si>
+    <t>Bildbereich</t>
+  </si>
+  <si>
+    <t>Linkobjekt</t>
+  </si>
+  <si>
+    <t>PDFDocument</t>
+  </si>
+  <si>
+    <t>PDF Document</t>
+  </si>
+  <si>
+    <t>PDF-Dokument</t>
+  </si>
+  <si>
+    <t>hasComment</t>
+  </si>
+  <si>
+    <t>isAnnotationOf</t>
+  </si>
+  <si>
+    <t>hasLinkTo</t>
+  </si>
+  <si>
+    <t>hasColor</t>
+  </si>
+  <si>
+    <t>isRegionOf</t>
+  </si>
+  <si>
+    <t>hasGeometry</t>
+  </si>
+  <si>
+    <t>StillImageRepresentation</t>
   </si>
 </sst>
 </file>
@@ -456,7 +584,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,6 +610,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +630,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -797,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7011A-D3D9-4EA8-AB3C-BA62FE335401}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -815,228 +944,709 @@
     <col min="9" max="9" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="D1" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="G1" s="12" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="I1" s="12" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J1" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>20</v>
+        <v>122</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>20</v>
+        <v>127</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="F2" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" t="s">
+        <v>121</v>
+      </c>
+      <c r="L2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3" t="s">
+        <v>128</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" t="s">
+        <v>129</v>
+      </c>
+      <c r="G4" t="s">
+        <v>76</v>
+      </c>
+      <c r="H4" t="s">
         <v>82</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I4" t="s">
         <v>88</v>
-      </c>
-      <c r="I2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" t="s">
-        <v>96</v>
       </c>
       <c r="J4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H5" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="I5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="J5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L5" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="F6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="I6" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D7" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>130</v>
       </c>
       <c r="F7" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="H7" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="I7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="J7" t="s">
         <v>19</v>
+      </c>
+      <c r="K7" t="s">
+        <v>120</v>
+      </c>
+      <c r="L7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" t="s">
+        <v>102</v>
+      </c>
+      <c r="J8" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" t="s">
+        <v>103</v>
+      </c>
+      <c r="J9" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="J10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G11" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="J12" t="s">
+        <v>109</v>
+      </c>
+      <c r="K12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C13" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>110</v>
+      </c>
+      <c r="J13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>134</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>136</v>
+      </c>
+      <c r="B15" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" t="s">
+        <v>138</v>
+      </c>
+      <c r="F15" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" t="s">
+        <v>138</v>
+      </c>
+      <c r="J15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" t="s">
+        <v>120</v>
+      </c>
+      <c r="J16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>121</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="E17" t="s">
+        <v>120</v>
+      </c>
+      <c r="G17" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" t="s">
+        <v>121</v>
+      </c>
+      <c r="J17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F18" t="s">
+        <v>120</v>
+      </c>
+      <c r="G18" t="s">
+        <v>120</v>
+      </c>
+      <c r="I18" t="s">
+        <v>121</v>
+      </c>
+      <c r="J18" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E61EA9F-2919-1B44-B6DA-5D0B65C0525B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AC4931-01C1-8140-8A2B-4D533EF89169}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529F0DCB-3465-1B45-82EA-8011AF2852E6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4503CF-228D-6144-A49E-C6F9E3C47277}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C75235-A3E4-404F-8079-B7256781B3ED}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682BF4B4-868D-8247-BACC-4C766C6E1331}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1050,7 +1660,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1082,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1090,7 +1700,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1098,7 +1708,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1106,7 +1716,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1114,7 +1724,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1122,7 +1732,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1130,7 +1740,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1146,7 +1756,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1154,7 +1764,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C12"/>
     </row>
@@ -1163,7 +1773,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C13"/>
     </row>
@@ -1193,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5419B217-D9EC-F346-8233-C40615A8948C}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1206,81 +1816,81 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
+        <v>118</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>114</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1290,7 +1900,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1298,7 +1908,25 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1331,7 +1959,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1341,50 +1969,50 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1392,115 +2020,115 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1508,7 +2136,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1516,7 +2144,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1557,20 +2185,20 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1580,7 +2208,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1590,7 +2218,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1600,7 +2228,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1610,7 +2238,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1630,7 +2258,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1650,7 +2278,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1660,7 +2288,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1668,7 +2296,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1707,10 +2335,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1728,7 +2356,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1738,7 +2366,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1748,7 +2376,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1758,7 +2386,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1768,7 +2396,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1788,7 +2416,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1808,7 +2436,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1818,7 +2446,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1826,7 +2454,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1855,7 +2483,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1865,16 +2493,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1884,10 +2512,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -1897,7 +2525,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1905,10 +2533,72 @@
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D91115-9643-C84D-8DE4-4276C702C3EC}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBDFF79-AB37-3541-A8C9-534BFC0AEF1C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
shorten testdata files hardcode expectations
</commit_message>
<xml_diff>
--- a/testdata/Resources.xlsx
+++ b/testdata/Resources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA887E1B-BB51-AF4A-9B53-C3825F596F09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DE6B70-0C76-E54F-A2D5-378581D8981F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="8" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="156">
   <si>
     <t>Cardinality</t>
   </si>
@@ -498,6 +498,15 @@
   </si>
   <si>
     <t>Only Romansh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-N  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0-1   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1  </t>
   </si>
 </sst>
 </file>
@@ -593,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,6 +629,7 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7011A-D3D9-4EA8-AB3C-BA62FE335401}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1497,6 +1507,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1733,9 +1744,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1775,15 +1786,15 @@
         <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>54</v>
+      <c r="B5" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1791,7 +1802,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1799,7 +1810,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fix(excel2resources, excel2properties): cover all cases (DEV-1040) (#201)
* fix bugs, make code more robust
* PR-title: allow commas and numbers in scope
* fix DeprecationWarning in JSON Schema validation
* allow multiple superclasses for properties, add column 'gui_attributes'
* cover more cases in the test data
* add Romansh
</commit_message>
<xml_diff>
--- a/testdata/Resources.xlsx
+++ b/testdata/Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrivoal/Git-projets/medialitterature/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nusjoh00-adm/Desktop/dsp-tools/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E269DD2A-5CC0-834D-8DA7-E68A09DDFCBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54DE6B70-0C76-E54F-A2D5-378581D8981F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25480" yWindow="500" windowWidth="25720" windowHeight="28300" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="1" xr2:uid="{7DA9512F-9D5C-45E8-B143-D0C99717614D}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="8" r:id="rId1"/>
@@ -20,6 +20,14 @@
     <sheet name="FamilyMember" sheetId="5" r:id="rId5"/>
     <sheet name="MentionedPerson" sheetId="6" r:id="rId6"/>
     <sheet name="Alias" sheetId="7" r:id="rId7"/>
+    <sheet name="Image" sheetId="9" r:id="rId8"/>
+    <sheet name="Video" sheetId="10" r:id="rId9"/>
+    <sheet name="Audio" sheetId="11" r:id="rId10"/>
+    <sheet name="ZIP" sheetId="12" r:id="rId11"/>
+    <sheet name="PDFDocument" sheetId="13" r:id="rId12"/>
+    <sheet name="Annotation" sheetId="14" r:id="rId13"/>
+    <sheet name="LinkObject" sheetId="15" r:id="rId14"/>
+    <sheet name="RegionOfImage" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="156">
   <si>
     <t>Cardinality</t>
   </si>
@@ -93,24 +101,12 @@
     <t>Resource</t>
   </si>
   <si>
-    <t>Owner</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>property</t>
   </si>
   <si>
     <t>cardinality</t>
   </si>
   <si>
-    <t>isTitle</t>
-  </si>
-  <si>
-    <t>isTitleInEnglish</t>
-  </si>
-  <si>
     <t>isTitleInFrench</t>
   </si>
   <si>
@@ -132,12 +128,6 @@
     <t>isPlaceRelatedTo</t>
   </si>
   <si>
-    <t>GenericAnthroponym</t>
-  </si>
-  <si>
-    <t>Generic anthroponym</t>
-  </si>
-  <si>
     <t>isGenericAnthroponym</t>
   </si>
   <si>
@@ -204,12 +194,6 @@
     <t>Mentioned person</t>
   </si>
   <si>
-    <t>property_name</t>
-  </si>
-  <si>
-    <t>cadinality</t>
-  </si>
-  <si>
     <t>Alias</t>
   </si>
   <si>
@@ -249,90 +233,21 @@
     <t>comment_fr</t>
   </si>
   <si>
-    <t>I had established myself for several months in a central city in one of our southern departments, whose shore is bathed by the Mediterranean, and I was desirous of purchasing a country place in that marvellously picturesque land. </t>
-  </si>
-  <si>
-    <t>I had already looked at several pieces of property when, one day, the notary, who had been giving me some necessary directions for one of my explorations, said to me:</t>
-  </si>
-  <si>
-    <t>I have just received notice that at about eight leagues from here, in one of the most beautiful situations in the world, neither too far nor too near to the sea, there is a country house for sale.</t>
-  </si>
-  <si>
-    <t>I know nothing of it whatever; but if you would like to see it, monsieur, here are the precise directions how to find it. </t>
-  </si>
-  <si>
-    <t>You will have to arrange the affair with the curé of the village of ——."</t>
-  </si>
-  <si>
     <t>de</t>
   </si>
   <si>
     <t>it</t>
   </si>
   <si>
-    <t>A strange chance put me in possession of this journal.</t>
-  </si>
-  <si>
     <t>comment_de</t>
   </si>
   <si>
     <t>comment_it</t>
   </si>
   <si>
-    <t xml:space="preserve">Ein seltsamer Zufall brachte mich in den Besitz dieses Tagebuchs.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich hatte mich für einige Monate in einer Stadt im Zentrum eines unserer südlichen Departements niedergelassen, dessen Ufer vom Mittelmeer umspült wird, und wollte ein Grundstück in diesem wunderbar malerischen Land erwerben. </t>
-  </si>
-  <si>
-    <t>Ich hatte bereits mehrere Grundstücke besichtigt, als eines Tages der Notar, der mir die notwendigen Anweisungen für eine meiner Erkundungen gegeben hatte, zu mir sagte:</t>
-  </si>
-  <si>
-    <t>Ich habe soeben erfahren, dass etwa acht Meilen von hier, in einer der schönsten Lagen der Welt, weder zu weit noch zu nah am Meer, ein Landhaus zum Verkauf steht.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ich weiß nichts davon, aber wenn Sie es sehen möchten, Monsieur, finden Sie hier die genaue Wegbeschreibung. </t>
-  </si>
-  <si>
-    <t>Sie werden die Angelegenheit mit dem Pfarrer des Dorfes -- regeln müssen."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un étrange hasard m'a mis en possession de ce journal.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je m'étais établi depuis plusieurs mois dans une ville centrale d'un de nos départements méridionaux, dont le rivage est baigné par la Méditerranée, et je désirais acheter une maison de campagne dans cette contrée merveilleusement pittoresque. </t>
-  </si>
-  <si>
-    <t>J'avais déjà examiné plusieurs propriétés quand, un jour, le notaire, qui me donnait des indications nécessaires pour une de mes explorations, me dit :</t>
-  </si>
-  <si>
-    <t>Je viens de recevoir avis qu'à huit lieues d'ici environ, dans une des plus belles situations du monde, ni trop loin ni trop près de la mer, il y a une maison de campagne à vendre.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Je n'en sais rien du tout ; mais si vous voulez la voir, monsieur, voici les indications précises pour la trouver. </t>
-  </si>
-  <si>
-    <t>Vous devrez arranger l'affaire avec le curé du village de --."</t>
-  </si>
-  <si>
     <t xml:space="preserve">Uno strano caso mi mise in possesso di questo diario.  </t>
   </si>
   <si>
-    <t xml:space="preserve">Mi ero stabilito da diversi mesi in una città centrale di uno dei nostri dipartimenti del sud, la cui riva è bagnata dal Mediterraneo, e desideravo acquistare un posto in campagna in quella terra meravigliosamente pittoresca. </t>
-  </si>
-  <si>
-    <t>Avevo già visto diverse proprietà quando un giorno il notaio, che mi aveva dato alcune indicazioni necessarie per una delle mie esplorazioni, mi disse</t>
-  </si>
-  <si>
-    <t>Ho appena ricevuto la notizia che a circa otto leghe da qui, in una delle situazioni più belle del mondo, né troppo lontano né troppo vicino al mare, c'è una casa di campagna in vendita.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non ne so nulla; ma se volete vederla, signore, eccovi le indicazioni precise per trovarla. </t>
-  </si>
-  <si>
-    <t>Dovrete organizzare l'affare con il curato del villaggio di --".</t>
-  </si>
-  <si>
     <t>Proprietario</t>
   </si>
   <si>
@@ -345,9 +260,6 @@
     <t>Membro della famiglia</t>
   </si>
   <si>
-    <t>Persona menzionata</t>
-  </si>
-  <si>
     <t>Eigentümer</t>
   </si>
   <si>
@@ -361,6 +273,240 @@
   </si>
   <si>
     <t>Erwähnte Person</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Bild</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>MovingImageRepresentation</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>AudioRepresentation</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>ArchiveRepresentation</t>
+  </si>
+  <si>
+    <t>DocumentRepresentation</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>LinkObj</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>1-N</t>
+  </si>
+  <si>
+    <t>0-N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">isTitle  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> isTitleInEnglish </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Title </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  GenericAnthroponym  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generic anthroponym </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Title</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Owner  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alias  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Persona menzionata  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resource  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resource</t>
+  </si>
+  <si>
+    <t>LinkObject</t>
+  </si>
+  <si>
+    <t>Link Object</t>
+  </si>
+  <si>
+    <t>RegionOfImage</t>
+  </si>
+  <si>
+    <t>Region of an image</t>
+  </si>
+  <si>
+    <t>Bildbereich</t>
+  </si>
+  <si>
+    <t>Linkobjekt</t>
+  </si>
+  <si>
+    <t>PDFDocument</t>
+  </si>
+  <si>
+    <t>PDF Document</t>
+  </si>
+  <si>
+    <t>PDF-Dokument</t>
+  </si>
+  <si>
+    <t>hasComment</t>
+  </si>
+  <si>
+    <t>isAnnotationOf</t>
+  </si>
+  <si>
+    <t>hasLinkTo</t>
+  </si>
+  <si>
+    <t>hasColor</t>
+  </si>
+  <si>
+    <t>isRegionOf</t>
+  </si>
+  <si>
+    <t>hasGeometry</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>because</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>missing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">             </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Resource , dcterms:fantasy   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Resource   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">StillImageRepresentation, dcterms:image  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  isOwnerOf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correspondsToGenericAnthroponym    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   hasAnthroponym   </t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>comment_rm</t>
+  </si>
+  <si>
+    <t>Rumantsch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      </t>
+  </si>
+  <si>
+    <t>Only Rumantsch</t>
+  </si>
+  <si>
+    <t>Only English</t>
+  </si>
+  <si>
+    <t>Only German</t>
+  </si>
+  <si>
+    <t>Only French</t>
+  </si>
+  <si>
+    <t>Only Italian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  A strange chance put me in possession of this journal.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ein seltsamer Zufall brachte mich in den Besitz dieses Tagebuchs.    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Un étrange hasard m'a mis en possession de ce journal.</t>
+  </si>
+  <si>
+    <t>Only Romansh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-N  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   0-1   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1  </t>
   </si>
 </sst>
 </file>
@@ -456,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,6 +628,8 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,7 +649,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -797,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFB7011A-D3D9-4EA8-AB3C-BA62FE335401}">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -808,235 +956,783 @@
     <col min="1" max="2" width="20.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" customWidth="1"/>
     <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="5" max="6" width="18.33203125" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="J1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G2" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" t="s">
+        <v>150</v>
+      </c>
+      <c r="I2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" t="s">
+        <v>141</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="M2" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="N3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" t="s">
+        <v>146</v>
+      </c>
+      <c r="L4" t="s">
+        <v>107</v>
+      </c>
+      <c r="M4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
+      <c r="L5" t="s">
+        <v>134</v>
+      </c>
+      <c r="N5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="E1" s="12" t="s">
+      <c r="D6" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K7" t="s">
+        <v>152</v>
+      </c>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7" t="s">
+        <v>97</v>
+      </c>
+      <c r="N7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="G1" s="12" t="s">
+      <c r="B8" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="G8" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" t="s">
+        <v>79</v>
+      </c>
+      <c r="L8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" s="12" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" t="s">
+        <v>80</v>
+      </c>
+      <c r="H9" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" t="s">
         <v>81</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="M9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" t="s">
+        <v>147</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" t="s">
+        <v>83</v>
+      </c>
+      <c r="M10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="D11" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" t="s">
+        <v>148</v>
+      </c>
+      <c r="G11" t="s">
+        <v>84</v>
+      </c>
+      <c r="H11" t="s">
+        <v>84</v>
+      </c>
+      <c r="K11" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="K12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L12" t="s">
+        <v>86</v>
+      </c>
+      <c r="M12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>87</v>
+      </c>
+      <c r="L13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>109</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K14" t="s">
+        <v>98</v>
+      </c>
+      <c r="L14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" t="s">
+        <v>143</v>
+      </c>
+      <c r="L15" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="D16" t="s">
+        <v>126</v>
+      </c>
+      <c r="E16" t="s">
+        <v>127</v>
+      </c>
+      <c r="H16" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" t="s">
+        <v>142</v>
+      </c>
+      <c r="L16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E17" t="s">
+        <v>126</v>
+      </c>
+      <c r="H17" t="s">
+        <v>97</v>
+      </c>
+      <c r="I17" t="s">
+        <v>98</v>
+      </c>
+      <c r="L17" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G18" t="s">
+        <v>97</v>
+      </c>
+      <c r="H18" t="s">
+        <v>97</v>
+      </c>
+      <c r="J18" t="s">
+        <v>98</v>
+      </c>
+      <c r="L18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D19" t="s">
+        <v>130</v>
+      </c>
+      <c r="E19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" t="s">
+        <v>129</v>
+      </c>
+      <c r="L20" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>128</v>
+      </c>
+      <c r="D21" t="s">
+        <v>98</v>
+      </c>
+      <c r="I21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E61EA9F-2919-1B44-B6DA-5D0B65C0525B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39AC4931-01C1-8140-8A2B-4D533EF89169}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" t="s">
-        <v>94</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="6" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529F0DCB-3465-1B45-82EA-8011AF2852E6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="F3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I3" t="s">
-        <v>95</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4503CF-228D-6144-A49E-C6F9E3C47277}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45C75235-A3E4-404F-8079-B7256781B3ED}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{682BF4B4-868D-8247-BACC-4C766C6E1331}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" t="s">
-        <v>67</v>
-      </c>
-      <c r="E4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F4" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" t="s">
-        <v>90</v>
-      </c>
-      <c r="I4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>103</v>
-      </c>
-      <c r="F5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" t="s">
-        <v>85</v>
-      </c>
-      <c r="H5" t="s">
-        <v>91</v>
-      </c>
-      <c r="I5" t="s">
-        <v>97</v>
-      </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" t="s">
-        <v>86</v>
-      </c>
-      <c r="H6" t="s">
-        <v>92</v>
-      </c>
-      <c r="I6" t="s">
-        <v>98</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" t="s">
-        <v>76</v>
-      </c>
-      <c r="G7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H7" t="s">
-        <v>93</v>
-      </c>
-      <c r="I7" t="s">
-        <v>99</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
+        <v>118</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1046,11 +1742,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3015D75-1C5B-4AD1-9C97-0CD088290370}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1071,7 +1767,7 @@
     </row>
     <row r="2" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>3</v>
+        <v>138</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
@@ -1079,26 +1775,26 @@
     </row>
     <row r="3" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>136</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>5</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>62</v>
+      <c r="B5" s="14" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1106,7 +1802,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1114,7 +1810,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1122,7 +1818,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>1</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1130,7 +1826,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -1146,7 +1842,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1154,7 +1850,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C12"/>
     </row>
@@ -1163,7 +1859,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C13"/>
     </row>
@@ -1184,6 +1880,29 @@
         <v>1</v>
       </c>
       <c r="C15"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>129</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1193,10 +1912,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5419B217-D9EC-F346-8233-C40615A8948C}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1206,81 +1925,81 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>25</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1290,7 +2009,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1298,7 +2017,25 @@
         <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1331,7 +2068,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1341,50 +2078,50 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1392,115 +2129,115 @@
         <v>7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1508,7 +2245,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1516,7 +2253,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1557,20 +2294,20 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1580,7 +2317,7 @@
         <v>5</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1590,7 +2327,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1600,7 +2337,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1610,7 +2347,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -1630,7 +2367,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -1650,7 +2387,7 @@
         <v>12</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1660,7 +2397,7 @@
         <v>13</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1668,7 +2405,7 @@
         <v>14</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1697,7 +2434,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1707,10 +2444,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1728,7 +2465,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1738,7 +2475,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -1748,7 +2485,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1758,7 +2495,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1768,7 +2505,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1788,7 +2525,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -1808,7 +2545,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -1818,7 +2555,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1826,7 +2563,7 @@
         <v>14</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1855,7 +2592,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1865,16 +2602,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1884,10 +2621,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11"/>
@@ -1897,7 +2634,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1905,10 +2642,72 @@
         <v>7</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D91115-9643-C84D-8DE4-4276C702C3EC}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EBDFF79-AB37-3541-A8C9-534BFC0AEF1C}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>